<commit_message>
update for GSTT data
account for double CBCT dates
identifying scan via medical system taken on
</commit_message>
<xml_diff>
--- a/Contour_Naming.xlsx
+++ b/Contour_Naming.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\poppy\Documents\RTSTRUCT_conversion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Poppy\Downloads\rtstruct_conversion-main\rtstruct_conversion-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9408ECDB-2662-4A2B-AFC0-CEECCDE1182F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5852E41-EFCB-43FA-9C16-2FFAB77E2C56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20010" yWindow="270" windowWidth="17280" windowHeight="11970" xr2:uid="{5DF877E1-B13A-4E63-BEA5-8EBCBDF21B0C}"/>
+    <workbookView xWindow="25080" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{5DF877E1-B13A-4E63-BEA5-8EBCBDF21B0C}"/>
   </bookViews>
   <sheets>
     <sheet name="H&amp;N" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="72">
   <si>
     <t>CTVLOW</t>
   </si>
@@ -219,6 +219,39 @@
   </si>
   <si>
     <t>couchsurface</t>
+  </si>
+  <si>
+    <t>parotid_l</t>
+  </si>
+  <si>
+    <t>parotid_r</t>
+  </si>
+  <si>
+    <t>spinalcord</t>
+  </si>
+  <si>
+    <t>CTV60</t>
+  </si>
+  <si>
+    <t>CTV54combi</t>
+  </si>
+  <si>
+    <t>Parotid_L</t>
+  </si>
+  <si>
+    <t>Parotid_R</t>
+  </si>
+  <si>
+    <t>CTVp</t>
+  </si>
+  <si>
+    <t>CTVn</t>
+  </si>
+  <si>
+    <t>CTV1</t>
+  </si>
+  <si>
+    <t>CTV2</t>
   </si>
 </sst>
 </file>
@@ -579,21 +612,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C8B3F16-A965-4D6D-ADE4-F0255756CE23}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="I1" sqref="I1:K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="11" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" customWidth="1"/>
-    <col min="6" max="6" width="10.5546875" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -619,7 +653,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -644,8 +678,10 @@
       <c r="H2" s="1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -668,7 +704,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -691,7 +727,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -711,7 +747,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -728,7 +764,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -745,7 +781,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -755,8 +791,14 @@
       <c r="D8" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -766,16 +808,25 @@
       <c r="D9" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E9" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D10" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -783,7 +834,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -791,7 +842,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -799,7 +850,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -807,12 +858,36 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>